<commit_message>
fix the urls due to the update of wikipedia
</commit_message>
<xml_diff>
--- a/xlsx/游戏_intext.xlsx
+++ b/xlsx/游戏_intext.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="351">
   <si>
     <t>游戏</t>
   </si>
@@ -954,6 +954,30 @@
   </si>
   <si>
     <t>临场动态角色扮演游戏</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/%E5%A4%9A%E4%BA%BA%E5%9C%A8%E7%BA%BF%E6%88%98%E6%96%97%E7%AB%9E%E6%8A%80%E5%9C%BA%E6%B8%B8%E6%88%8F</t>
+  </si>
+  <si>
+    <t>多人在线战斗竞技场游戏</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/%E9%AD%94%E5%85%BD%E4%BA%89%E9%9C%B8III%EF%BC%9A%E6%B7%B7%E4%B9%B1%E4%B9%8B%E6%B2%BB</t>
+  </si>
+  <si>
+    <t>魔兽争霸III：混乱之治</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/%E8%8B%B1%E9%9B%84%E8%81%94%E7%9B%9F</t>
+  </si>
+  <si>
+    <t>英雄联盟</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/DotA</t>
+  </si>
+  <si>
+    <t>DotA</t>
   </si>
   <si>
     <t>https://zh.wikipedia.org/wiki/%E7%9B%8A%E6%99%BA%E6%B8%B8%E6%88%8F</t>
@@ -1392,7 +1416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1562,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
@@ -6028,7 +6052,7 @@
         <v>314</v>
       </c>
       <c r="G160" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H160" t="s">
         <v>4</v>
@@ -6080,10 +6104,10 @@
         <v>161</v>
       </c>
       <c r="E162" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="F162" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="G162" t="n">
         <v>1</v>
@@ -6109,10 +6133,10 @@
         <v>162</v>
       </c>
       <c r="E163" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F163" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G163" t="n">
         <v>1</v>
@@ -6138,10 +6162,10 @@
         <v>163</v>
       </c>
       <c r="E164" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F164" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G164" t="n">
         <v>1</v>
@@ -6167,13 +6191,13 @@
         <v>164</v>
       </c>
       <c r="E165" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F165" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H165" t="s">
         <v>4</v>
@@ -6196,10 +6220,10 @@
         <v>165</v>
       </c>
       <c r="E166" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="F166" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="G166" t="n">
         <v>1</v>
@@ -6289,7 +6313,7 @@
         <v>330</v>
       </c>
       <c r="G169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H169" t="s">
         <v>4</v>
@@ -6434,7 +6458,7 @@
         <v>340</v>
       </c>
       <c r="G174" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H174" t="s">
         <v>4</v>
@@ -6469,6 +6493,122 @@
         <v>4</v>
       </c>
       <c r="I175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" t="s">
+        <v>1</v>
+      </c>
+      <c r="D176" t="n">
+        <v>175</v>
+      </c>
+      <c r="E176" t="s">
+        <v>343</v>
+      </c>
+      <c r="F176" t="s">
+        <v>344</v>
+      </c>
+      <c r="G176" t="n">
+        <v>1</v>
+      </c>
+      <c r="H176" t="s">
+        <v>4</v>
+      </c>
+      <c r="I176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" t="s">
+        <v>1</v>
+      </c>
+      <c r="D177" t="n">
+        <v>176</v>
+      </c>
+      <c r="E177" t="s">
+        <v>345</v>
+      </c>
+      <c r="F177" t="s">
+        <v>346</v>
+      </c>
+      <c r="G177" t="n">
+        <v>1</v>
+      </c>
+      <c r="H177" t="s">
+        <v>4</v>
+      </c>
+      <c r="I177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C178" t="s">
+        <v>1</v>
+      </c>
+      <c r="D178" t="n">
+        <v>177</v>
+      </c>
+      <c r="E178" t="s">
+        <v>347</v>
+      </c>
+      <c r="F178" t="s">
+        <v>348</v>
+      </c>
+      <c r="G178" t="n">
+        <v>2</v>
+      </c>
+      <c r="H178" t="s">
+        <v>4</v>
+      </c>
+      <c r="I178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>0</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1</v>
+      </c>
+      <c r="D179" t="n">
+        <v>178</v>
+      </c>
+      <c r="E179" t="s">
+        <v>349</v>
+      </c>
+      <c r="F179" t="s">
+        <v>350</v>
+      </c>
+      <c r="G179" t="n">
+        <v>1</v>
+      </c>
+      <c r="H179" t="s">
+        <v>4</v>
+      </c>
+      <c r="I179" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>